<commit_message>
final Project - source code edit
</commit_message>
<xml_diff>
--- a/testResponseData.xlsx
+++ b/testResponseData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박해영\Desktop\2018학년도 2학기\고급컴퓨터수학\PredictWineQuality_Matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8737CD44-DAFD-4290-820B-57FBE1FEE359}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6E76D66-B8B8-4F95-9EB3-CE37446CDC10}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10185" xr2:uid="{F76ED4A6-5FAD-4596-B837-4D8F58296520}"/>
   </bookViews>
@@ -421,12 +421,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
@@ -451,17 +451,17 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -471,37 +471,37 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
@@ -511,17 +511,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
@@ -546,12 +546,12 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -586,32 +586,32 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
@@ -621,22 +621,22 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
@@ -646,17 +646,17 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
@@ -666,12 +666,12 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
@@ -691,27 +691,27 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
@@ -721,22 +721,22 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
@@ -746,7 +746,7 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
@@ -756,7 +756,7 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
@@ -766,12 +766,12 @@
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
@@ -786,12 +786,12 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
@@ -811,7 +811,7 @@
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
@@ -821,12 +821,12 @@
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
@@ -841,7 +841,7 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
@@ -856,7 +856,7 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
@@ -866,12 +866,12 @@
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
@@ -896,7 +896,7 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
@@ -916,7 +916,7 @@
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
@@ -936,12 +936,12 @@
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
@@ -956,42 +956,42 @@
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
@@ -1016,7 +1016,7 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
@@ -1031,7 +1031,7 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
@@ -1041,22 +1041,22 @@
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
@@ -1066,62 +1066,62 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
@@ -1141,12 +1141,12 @@
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
@@ -1166,7 +1166,7 @@
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
@@ -1176,27 +1176,27 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
@@ -1206,17 +1206,17 @@
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
@@ -1231,17 +1231,17 @@
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
@@ -1251,17 +1251,17 @@
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
@@ -1276,12 +1276,12 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
@@ -1291,27 +1291,27 @@
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
@@ -1321,7 +1321,7 @@
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
@@ -1331,12 +1331,12 @@
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
@@ -1351,12 +1351,12 @@
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
@@ -1371,27 +1371,27 @@
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
@@ -1401,7 +1401,7 @@
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
@@ -1421,37 +1421,37 @@
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
@@ -1461,7 +1461,7 @@
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
@@ -1476,22 +1476,22 @@
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
@@ -1501,17 +1501,17 @@
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
@@ -1521,22 +1521,22 @@
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
@@ -1546,47 +1546,47 @@
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
@@ -1601,17 +1601,17 @@
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
@@ -1621,7 +1621,7 @@
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
@@ -1631,7 +1631,7 @@
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
@@ -1646,32 +1646,32 @@
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
@@ -1681,27 +1681,27 @@
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
@@ -1716,12 +1716,12 @@
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
@@ -1731,12 +1731,12 @@
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
@@ -1746,47 +1746,47 @@
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
@@ -1801,32 +1801,32 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
@@ -1836,7 +1836,7 @@
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
@@ -1856,17 +1856,17 @@
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
@@ -1876,12 +1876,12 @@
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
@@ -1891,7 +1891,7 @@
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
@@ -1906,37 +1906,37 @@
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
@@ -1951,7 +1951,7 @@
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
@@ -1961,7 +1961,7 @@
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
@@ -1971,32 +1971,32 @@
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
@@ -2006,17 +2006,17 @@
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
@@ -2026,7 +2026,7 @@
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
@@ -2036,17 +2036,17 @@
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
@@ -2056,12 +2056,12 @@
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
@@ -2071,7 +2071,7 @@
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
@@ -2081,17 +2081,17 @@
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
@@ -2106,7 +2106,7 @@
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
@@ -2116,17 +2116,17 @@
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
@@ -2141,12 +2141,12 @@
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.3">
@@ -2156,7 +2156,7 @@
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
@@ -2166,37 +2166,37 @@
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.3">
@@ -2206,17 +2206,17 @@
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
@@ -2226,17 +2226,17 @@
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.3">
@@ -2246,17 +2246,17 @@
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
@@ -2276,47 +2276,47 @@
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.3">
@@ -2326,37 +2326,37 @@
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.3">
@@ -2366,42 +2366,42 @@
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
@@ -2411,27 +2411,27 @@
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
@@ -2441,17 +2441,17 @@
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.3">
@@ -2461,7 +2461,7 @@
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.3">
@@ -2476,22 +2476,22 @@
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.3">
@@ -2501,17 +2501,17 @@
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.3">
@@ -2526,32 +2526,32 @@
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.3">
@@ -2566,42 +2566,42 @@
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.3">
@@ -2616,7 +2616,7 @@
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.3">
@@ -2626,17 +2626,17 @@
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
@@ -2651,22 +2651,22 @@
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.3">
@@ -2676,32 +2676,32 @@
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.3">
@@ -2711,17 +2711,17 @@
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.3">
@@ -2736,7 +2736,7 @@
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.3">
@@ -2751,17 +2751,17 @@
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.3">
@@ -2771,17 +2771,17 @@
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.3">
@@ -2791,17 +2791,17 @@
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A478">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.3">
@@ -2811,12 +2811,12 @@
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.3">
@@ -2826,12 +2826,12 @@
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A484">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.3">
@@ -2841,7 +2841,7 @@
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.3">
@@ -2851,27 +2851,27 @@
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A489">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.3">
@@ -2881,7 +2881,7 @@
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.3">
@@ -2896,12 +2896,12 @@
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.3">
@@ -2911,22 +2911,22 @@
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A503">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A504">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.3">
@@ -2936,7 +2936,7 @@
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.3">
@@ -2946,22 +2946,22 @@
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A508">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A509">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A510">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.3">
@@ -2981,12 +2981,12 @@
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A515">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A516">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.3">
@@ -3001,12 +3001,12 @@
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A519">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A520">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.3">
@@ -3016,7 +3016,7 @@
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A522">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.3">
@@ -3026,7 +3026,7 @@
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A524">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.3">
@@ -3036,22 +3036,22 @@
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A526">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A527">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A528">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A529">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.3">
@@ -3066,52 +3066,52 @@
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A533">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A534">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A535">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A536">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A537">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A538">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A539">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A540">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A541">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.3">
@@ -3131,27 +3131,27 @@
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A545">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A546">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A547">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A548">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A549">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.3">
@@ -3166,27 +3166,27 @@
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A552">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A553">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A554">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A555">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A556">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.3">
@@ -3201,22 +3201,22 @@
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A559">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A560">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A561">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A562">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.3">
@@ -3226,27 +3226,27 @@
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A564">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A565">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A566">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A567">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A568">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.3">
@@ -3256,7 +3256,7 @@
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A570">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.3">
@@ -3266,7 +3266,7 @@
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A572">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.3">
@@ -3276,27 +3276,27 @@
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A574">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A575">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A576">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A577">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A578">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.3">
@@ -3316,12 +3316,12 @@
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A582">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A583">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.3">
@@ -3336,22 +3336,22 @@
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A586">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A587">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A588">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A589">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.3">
@@ -3361,42 +3361,42 @@
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A591">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A592">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A593">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A594">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A595">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A596">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A597">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A598">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.3">
@@ -3406,27 +3406,27 @@
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A600">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A601">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A602">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A603">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A604">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.3">
@@ -3436,22 +3436,22 @@
     </row>
     <row r="606" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A606">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A607">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A608">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="609" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A609">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="610" spans="1:1" x14ac:dyDescent="0.3">
@@ -3461,7 +3461,7 @@
     </row>
     <row r="611" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A611">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="612" spans="1:1" x14ac:dyDescent="0.3">
@@ -3471,17 +3471,17 @@
     </row>
     <row r="613" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A613">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A614">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A615">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.3">
@@ -3491,22 +3491,22 @@
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A617">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A618">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A619">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A620">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.3">
@@ -3521,12 +3521,12 @@
     </row>
     <row r="623" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A623">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="624" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A624">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.3">
@@ -3546,7 +3546,7 @@
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A628">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.3">
@@ -3556,7 +3556,7 @@
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A630">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.3">
@@ -3566,17 +3566,17 @@
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A632">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A633">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A634">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.3">
@@ -3591,12 +3591,12 @@
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A637">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A638">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.3">
@@ -3606,12 +3606,12 @@
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A640">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A641">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.3">
@@ -3621,7 +3621,7 @@
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A643">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.3">
@@ -3631,7 +3631,7 @@
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A645">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.3">
@@ -3641,7 +3641,7 @@
     </row>
     <row r="647" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A647">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.3">
@@ -3666,7 +3666,7 @@
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A652">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.3">
@@ -3676,7 +3676,7 @@
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A654">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.3">
@@ -3686,47 +3686,47 @@
     </row>
     <row r="656" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A656">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A657">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A658">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A659">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A660">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A661">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A662">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A663">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A664">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.3">
@@ -3736,22 +3736,22 @@
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A666">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A667">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A668">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="669" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A669">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.3">
@@ -3761,22 +3761,22 @@
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A671">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A672">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A673">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A674">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.3">
@@ -3791,7 +3791,7 @@
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A677">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.3">
@@ -3811,7 +3811,7 @@
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A681">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.3">
@@ -3821,12 +3821,12 @@
     </row>
     <row r="683" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A683">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="684" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A684">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.3">
@@ -3841,7 +3841,7 @@
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A687">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.3">
@@ -3851,7 +3851,7 @@
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A689">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="690" spans="1:1" x14ac:dyDescent="0.3">
@@ -3861,12 +3861,12 @@
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A691">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A692">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="693" spans="1:1" x14ac:dyDescent="0.3">
@@ -3876,12 +3876,12 @@
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A694">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A695">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.3">
@@ -3891,17 +3891,17 @@
     </row>
     <row r="697" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A697">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="698" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A698">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="699" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A699">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="700" spans="1:1" x14ac:dyDescent="0.3">
@@ -3911,7 +3911,7 @@
     </row>
     <row r="701" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A701">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="702" spans="1:1" x14ac:dyDescent="0.3">
@@ -3921,17 +3921,17 @@
     </row>
     <row r="703" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A703">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="704" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A704">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="705" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A705">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.3">
@@ -3941,62 +3941,62 @@
     </row>
     <row r="707" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A707">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A708">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="709" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A709">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A710">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A711">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="712" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A712">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="713" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A713">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="714" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A714">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A715">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A716">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A717">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A718">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.3">
@@ -4011,7 +4011,7 @@
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A721">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="722" spans="1:1" x14ac:dyDescent="0.3">
@@ -4026,17 +4026,17 @@
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A724">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A725">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="726" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A726">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="727" spans="1:1" x14ac:dyDescent="0.3">
@@ -4061,7 +4061,7 @@
     </row>
     <row r="731" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A731">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.3">
@@ -4071,22 +4071,22 @@
     </row>
     <row r="733" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A733">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="734" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A734">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="735" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A735">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="736" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A736">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="737" spans="1:1" x14ac:dyDescent="0.3">
@@ -4106,7 +4106,7 @@
     </row>
     <row r="740" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A740">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="741" spans="1:1" x14ac:dyDescent="0.3">
@@ -4121,22 +4121,22 @@
     </row>
     <row r="743" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A743">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="744" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A744">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="745" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A745">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="746" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A746">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="747" spans="1:1" x14ac:dyDescent="0.3">
@@ -4146,7 +4146,7 @@
     </row>
     <row r="748" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A748">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="749" spans="1:1" x14ac:dyDescent="0.3">
@@ -4156,52 +4156,52 @@
     </row>
     <row r="750" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A750">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="751" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A751">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="752" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A752">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="753" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A753">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="754" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A754">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="755" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A755">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="756" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A756">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="757" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A757">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="758" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A758">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="759" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A759">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="760" spans="1:1" x14ac:dyDescent="0.3">
@@ -4216,77 +4216,77 @@
     </row>
     <row r="762" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A762">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="763" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A763">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="764" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A764">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="765" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A765">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="766" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A766">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="767" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A767">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="768" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A768">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="769" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A769">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A770">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="771" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A771">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A772">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A773">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="774" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A774">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="775" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A775">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="776" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A776">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="777" spans="1:1" x14ac:dyDescent="0.3">
@@ -4306,17 +4306,17 @@
     </row>
     <row r="780" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A780">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="781" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A781">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="782" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A782">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="783" spans="1:1" x14ac:dyDescent="0.3">
@@ -4331,7 +4331,7 @@
     </row>
     <row r="785" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A785">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="786" spans="1:1" x14ac:dyDescent="0.3">
@@ -4346,22 +4346,22 @@
     </row>
     <row r="788" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A788">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="789" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A789">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="790" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A790">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="791" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A791">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="792" spans="1:1" x14ac:dyDescent="0.3">
@@ -4371,32 +4371,32 @@
     </row>
     <row r="793" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A793">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="794" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A794">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="795" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A795">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="796" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A796">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="797" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A797">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="798" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A798">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="799" spans="1:1" x14ac:dyDescent="0.3">
@@ -4416,37 +4416,37 @@
     </row>
     <row r="802" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A802">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="803" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A803">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="804" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A804">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="805" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A805">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="806" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A806">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="807" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A807">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="808" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A808">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="809" spans="1:1" x14ac:dyDescent="0.3">
@@ -4471,7 +4471,7 @@
     </row>
     <row r="813" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A813">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="814" spans="1:1" x14ac:dyDescent="0.3">
@@ -4481,7 +4481,7 @@
     </row>
     <row r="815" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A815">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="816" spans="1:1" x14ac:dyDescent="0.3">
@@ -4491,12 +4491,12 @@
     </row>
     <row r="817" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A817">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="818" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A818">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="819" spans="1:1" x14ac:dyDescent="0.3">
@@ -4506,17 +4506,17 @@
     </row>
     <row r="820" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A820">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="821" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A821">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="822" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A822">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="823" spans="1:1" x14ac:dyDescent="0.3">
@@ -4536,7 +4536,7 @@
     </row>
     <row r="826" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A826">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="827" spans="1:1" x14ac:dyDescent="0.3">
@@ -4546,27 +4546,27 @@
     </row>
     <row r="828" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A828">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="829" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A829">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="830" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A830">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="831" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A831">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="832" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A832">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="833" spans="1:1" x14ac:dyDescent="0.3">
@@ -4581,12 +4581,12 @@
     </row>
     <row r="835" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A835">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="836" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A836">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="837" spans="1:1" x14ac:dyDescent="0.3">
@@ -4606,17 +4606,17 @@
     </row>
     <row r="840" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A840">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="841" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A841">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="842" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A842">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="843" spans="1:1" x14ac:dyDescent="0.3">
@@ -4636,7 +4636,7 @@
     </row>
     <row r="846" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A846">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="847" spans="1:1" x14ac:dyDescent="0.3">
@@ -4651,12 +4651,12 @@
     </row>
     <row r="849" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A849">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="850" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A850">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="851" spans="1:1" x14ac:dyDescent="0.3">
@@ -4666,22 +4666,22 @@
     </row>
     <row r="852" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A852">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="853" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A853">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="854" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A854">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="855" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A855">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="856" spans="1:1" x14ac:dyDescent="0.3">
@@ -4691,7 +4691,7 @@
     </row>
     <row r="857" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A857">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="858" spans="1:1" x14ac:dyDescent="0.3">
@@ -4701,12 +4701,12 @@
     </row>
     <row r="859" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A859">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="860" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A860">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="861" spans="1:1" x14ac:dyDescent="0.3">
@@ -4716,12 +4716,12 @@
     </row>
     <row r="862" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A862">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="863" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A863">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="864" spans="1:1" x14ac:dyDescent="0.3">
@@ -4731,7 +4731,7 @@
     </row>
     <row r="865" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A865">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="866" spans="1:1" x14ac:dyDescent="0.3">
@@ -4751,22 +4751,22 @@
     </row>
     <row r="869" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A869">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="870" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A870">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="871" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A871">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="872" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A872">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="873" spans="1:1" x14ac:dyDescent="0.3">
@@ -4776,7 +4776,7 @@
     </row>
     <row r="874" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A874">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="875" spans="1:1" x14ac:dyDescent="0.3">
@@ -4786,12 +4786,12 @@
     </row>
     <row r="876" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A876">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="877" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A877">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="878" spans="1:1" x14ac:dyDescent="0.3">
@@ -4801,7 +4801,7 @@
     </row>
     <row r="879" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A879">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="880" spans="1:1" x14ac:dyDescent="0.3">
@@ -4811,7 +4811,7 @@
     </row>
     <row r="881" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A881">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="882" spans="1:1" x14ac:dyDescent="0.3">
@@ -4821,12 +4821,12 @@
     </row>
     <row r="883" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A883">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="884" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A884">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="885" spans="1:1" x14ac:dyDescent="0.3">
@@ -4841,12 +4841,12 @@
     </row>
     <row r="887" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A887">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="888" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A888">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="889" spans="1:1" x14ac:dyDescent="0.3">
@@ -4861,12 +4861,12 @@
     </row>
     <row r="891" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A891">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="892" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A892">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="893" spans="1:1" x14ac:dyDescent="0.3">
@@ -4876,7 +4876,7 @@
     </row>
     <row r="894" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A894">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="895" spans="1:1" x14ac:dyDescent="0.3">
@@ -4891,27 +4891,27 @@
     </row>
     <row r="897" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A897">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="898" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A898">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="899" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A899">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="900" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A900">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="901" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A901">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="902" spans="1:1" x14ac:dyDescent="0.3">
@@ -4921,7 +4921,7 @@
     </row>
     <row r="903" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A903">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="904" spans="1:1" x14ac:dyDescent="0.3">
@@ -4931,32 +4931,32 @@
     </row>
     <row r="905" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A905">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="906" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A906">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="907" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A907">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="908" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A908">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="909" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A909">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="910" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A910">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="911" spans="1:1" x14ac:dyDescent="0.3">
@@ -4966,7 +4966,7 @@
     </row>
     <row r="912" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A912">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="913" spans="1:1" x14ac:dyDescent="0.3">
@@ -4976,7 +4976,7 @@
     </row>
     <row r="914" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A914">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="915" spans="1:1" x14ac:dyDescent="0.3">
@@ -4986,7 +4986,7 @@
     </row>
     <row r="916" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A916">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="917" spans="1:1" x14ac:dyDescent="0.3">
@@ -4996,7 +4996,7 @@
     </row>
     <row r="918" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A918">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="919" spans="1:1" x14ac:dyDescent="0.3">
@@ -5006,32 +5006,32 @@
     </row>
     <row r="920" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A920">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="921" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A921">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="922" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A922">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="923" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A923">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="924" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A924">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="925" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A925">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="926" spans="1:1" x14ac:dyDescent="0.3">
@@ -5051,12 +5051,12 @@
     </row>
     <row r="929" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A929">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="930" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A930">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="931" spans="1:1" x14ac:dyDescent="0.3">
@@ -5071,22 +5071,22 @@
     </row>
     <row r="933" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A933">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="934" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A934">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="935" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A935">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="936" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A936">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="937" spans="1:1" x14ac:dyDescent="0.3">
@@ -5106,27 +5106,27 @@
     </row>
     <row r="940" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A940">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="941" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A941">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="942" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A942">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="943" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A943">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="944" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A944">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="945" spans="1:1" x14ac:dyDescent="0.3">
@@ -5136,7 +5136,7 @@
     </row>
     <row r="946" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A946">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="947" spans="1:1" x14ac:dyDescent="0.3">
@@ -5156,7 +5156,7 @@
     </row>
     <row r="950" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A950">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="951" spans="1:1" x14ac:dyDescent="0.3">
@@ -5166,7 +5166,7 @@
     </row>
     <row r="952" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A952">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="953" spans="1:1" x14ac:dyDescent="0.3">
@@ -5176,17 +5176,17 @@
     </row>
     <row r="954" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A954">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="955" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A955">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="956" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A956">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="957" spans="1:1" x14ac:dyDescent="0.3">
@@ -5201,12 +5201,12 @@
     </row>
     <row r="959" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A959">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="960" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A960">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="961" spans="1:1" x14ac:dyDescent="0.3">
@@ -5216,12 +5216,12 @@
     </row>
     <row r="962" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A962">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="963" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A963">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="964" spans="1:1" x14ac:dyDescent="0.3">
@@ -5231,32 +5231,32 @@
     </row>
     <row r="965" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A965">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="966" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A966">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="967" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A967">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="968" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A968">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="969" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A969">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="970" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A970">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="971" spans="1:1" x14ac:dyDescent="0.3">
@@ -5266,12 +5266,12 @@
     </row>
     <row r="972" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A972">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="973" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A973">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="974" spans="1:1" x14ac:dyDescent="0.3">
@@ -5281,12 +5281,12 @@
     </row>
     <row r="975" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A975">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="976" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A976">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="977" spans="1:1" x14ac:dyDescent="0.3">
@@ -5296,17 +5296,17 @@
     </row>
     <row r="978" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A978">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="979" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A979">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="980" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A980">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>